<commit_message>
Adding new property for researching key columns.
</commit_message>
<xml_diff>
--- a/TestExcelEntityMapper/Risorse/empty_XLSX.xlsx
+++ b/TestExcelEntityMapper/Risorse/empty_XLSX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="11100" windowHeight="6705" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="11100" windowHeight="6705"/>
   </bookViews>
   <sheets>
     <sheet name="Persons" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -36,6 +36,21 @@
   </si>
   <si>
     <t>OwnCar.BuildYear</t>
+  </si>
+  <si>
+    <t>pippo</t>
+  </si>
+  <si>
+    <t>pluto</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>DQ789AQ</t>
   </si>
 </sst>
 </file>
@@ -50,14 +65,12 @@
     </font>
     <font>
       <b/>
-      <u/>
       <sz val="10"/>
       <name val="SansSerif"/>
       <charset val="1"/>
     </font>
     <font>
       <b/>
-      <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Consolas"/>
@@ -90,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -104,6 +117,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -399,10 +414,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="B2:H5"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -411,46 +426,58 @@
     <col min="4" max="4" width="29.85546875" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="2:8">
       <c r="D2" s="2"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
-      <c r="D3" s="2"/>
-      <c r="G3" s="1"/>
+    <row r="4" spans="2:8">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="D4" s="2"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="D5" s="2"/>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5">
+        <v>29504</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="6">
+        <v>2009</v>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -467,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>

</xml_diff>

<commit_message>
Improvement unit test project
</commit_message>
<xml_diff>
--- a/TestExcelEntityMapper/Risorse/empty_XLSX.xlsx
+++ b/TestExcelEntityMapper/Risorse/empty_XLSX.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="11100" windowHeight="6705"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="11100" windowHeight="6705" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Persons" sheetId="2" r:id="rId1"/>
     <sheet name="Persons2" sheetId="3" r:id="rId2"/>
+    <sheet name="Persons3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -51,6 +52,15 @@
   </si>
   <si>
     <t>DQ789AQ</t>
+  </si>
+  <si>
+    <t>QY478AZ</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>Ford demo</t>
   </si>
 </sst>
 </file>
@@ -416,7 +426,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" workbookViewId="0">
+    <sheetView showOutlineSymbols="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:H5"/>
     </sheetView>
   </sheetViews>
@@ -492,9 +502,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B8:N9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="8" spans="2:14">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5">
+        <v>29504</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="6">
+        <v>2009</v>
+      </c>
+      <c r="L8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="L9" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>

</xml_diff>

<commit_message>
New implementations for reading data source.
</commit_message>
<xml_diff>
--- a/TestExcelEntityMapper/Risorse/empty_XLSX.xlsx
+++ b/TestExcelEntityMapper/Risorse/empty_XLSX.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="11100" windowHeight="6705" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="11100" windowHeight="6705" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Persons" sheetId="2" r:id="rId1"/>
     <sheet name="Persons2" sheetId="3" r:id="rId2"/>
     <sheet name="Persons3" sheetId="4" r:id="rId3"/>
+    <sheet name="Persons4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -427,7 +428,7 @@
   <dimension ref="B2:H5"/>
   <sheetViews>
     <sheetView showOutlineSymbols="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H5"/>
+      <selection activeCell="B4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -555,10 +556,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B6:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:8">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New methods for mappers.
</commit_message>
<xml_diff>
--- a/TestExcelEntityMapper/Risorse/empty_XLSX.xlsx
+++ b/TestExcelEntityMapper/Risorse/empty_XLSX.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="11100" windowHeight="6705" activeTab="3"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -62,6 +62,18 @@
   </si>
   <si>
     <t>Ford demo</t>
+  </si>
+  <si>
+    <t>mario</t>
+  </si>
+  <si>
+    <t>gomez</t>
+  </si>
+  <si>
+    <t>Alfa</t>
+  </si>
+  <si>
+    <t>DD457ZA</t>
   </si>
 </sst>
 </file>
@@ -114,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -130,6 +142,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -425,10 +438,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:H5"/>
+  <dimension ref="B2:H6"/>
   <sheetViews>
     <sheetView showOutlineSymbols="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -490,6 +503,29 @@
         <v>2009</v>
       </c>
     </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>1989</v>
+      </c>
+      <c r="E6" s="7">
+        <v>25812</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>2008</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -506,7 +542,7 @@
   <dimension ref="B8:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -544,6 +580,27 @@
       </c>
     </row>
     <row r="9" spans="2:14">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>1989</v>
+      </c>
+      <c r="E9" s="7">
+        <v>25812</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>2008</v>
+      </c>
       <c r="L9" s="6"/>
     </row>
   </sheetData>

</xml_diff>